<commit_message>
Este es el segundo commit
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\prueba_camilo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FEDFF21-A52C-4E13-A1C6-8F279450E371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FEF558-B75B-4D28-A467-C748AC3E7B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{AC46AA12-DF18-44CA-ACC2-E9D8C515F945}"/>
   </bookViews>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F060172C-37CB-4B0A-BC5B-12A867E98C0E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +446,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Este es el tercer commit
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\prueba_camilo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FEF558-B75B-4D28-A467-C748AC3E7B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8423C9-41C5-4A67-BC8E-18850FFE9BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{AC46AA12-DF18-44CA-ACC2-E9D8C515F945}"/>
   </bookViews>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F060172C-37CB-4B0A-BC5B-12A867E98C0E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +457,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>